<commit_message>
build an iterator to test the normal long short strategy
</commit_message>
<xml_diff>
--- a/Python/trades_ETHUSDT_5m_complete_history_long_short.xlsx
+++ b/Python/trades_ETHUSDT_5m_complete_history_long_short.xlsx
@@ -50,6 +50,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -102,11 +105,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,14 +469,14 @@
       <c r="H2">
         <v>-0.01735456769235855</v>
       </c>
-      <c r="I2">
-        <v>3583</v>
-      </c>
-      <c r="J2">
-        <v>5599</v>
-      </c>
-      <c r="K2">
-        <v>2016</v>
+      <c r="I2" s="2">
+        <v>44268.50347222222</v>
+      </c>
+      <c r="J2" s="2">
+        <v>44275.50347222222</v>
+      </c>
+      <c r="K2" s="3">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -499,14 +504,14 @@
       <c r="H3">
         <v>0.1566503855536203</v>
       </c>
-      <c r="I3">
-        <v>8176</v>
-      </c>
-      <c r="J3">
-        <v>10192</v>
-      </c>
-      <c r="K3">
-        <v>2016</v>
+      <c r="I3" s="2">
+        <v>44284.45138888889</v>
+      </c>
+      <c r="J3" s="2">
+        <v>44291.45138888889</v>
+      </c>
+      <c r="K3" s="3">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -534,14 +539,14 @@
       <c r="H4">
         <v>0.1442362611174635</v>
       </c>
-      <c r="I4">
-        <v>11558</v>
-      </c>
-      <c r="J4">
-        <v>13574</v>
-      </c>
-      <c r="K4">
-        <v>2016</v>
+      <c r="I4" s="2">
+        <v>44296.19444444445</v>
+      </c>
+      <c r="J4" s="2">
+        <v>44303.19444444445</v>
+      </c>
+      <c r="K4" s="3">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -569,14 +574,14 @@
       <c r="H5">
         <v>0.06227657072874515</v>
       </c>
-      <c r="I5">
-        <v>19660</v>
-      </c>
-      <c r="J5">
-        <v>21676</v>
-      </c>
-      <c r="K5">
-        <v>2016</v>
+      <c r="I5" s="2">
+        <v>44324.625</v>
+      </c>
+      <c r="J5" s="2">
+        <v>44331.625</v>
+      </c>
+      <c r="K5" s="3">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -604,14 +609,14 @@
       <c r="H6">
         <v>0.3598437363063514</v>
       </c>
-      <c r="I6">
-        <v>22803</v>
-      </c>
-      <c r="J6">
-        <v>22837</v>
-      </c>
-      <c r="K6">
-        <v>34</v>
+      <c r="I6" s="2">
+        <v>44335.53819444445</v>
+      </c>
+      <c r="J6" s="2">
+        <v>44335.65625</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0.1180555555555556</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -625,28 +630,28 @@
         <v>22837</v>
       </c>
       <c r="D7">
-        <v>32122</v>
+        <v>24853</v>
       </c>
       <c r="E7">
         <v>2728.7685</v>
       </c>
       <c r="F7">
-        <v>2261.26</v>
+        <v>2744.51</v>
       </c>
       <c r="G7">
-        <v>2805.050999999999</v>
+        <v>-94.44900000000052</v>
       </c>
       <c r="H7">
-        <v>0.1713258196875257</v>
-      </c>
-      <c r="I7">
-        <v>22837</v>
-      </c>
-      <c r="J7">
-        <v>32122</v>
-      </c>
-      <c r="K7">
-        <v>9285</v>
+        <v>-0.005768719479134932</v>
+      </c>
+      <c r="I7" s="2">
+        <v>44335.65625</v>
+      </c>
+      <c r="J7" s="2">
+        <v>44342.65625</v>
+      </c>
+      <c r="K7" s="3">
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -654,7 +659,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>32122</v>
@@ -669,19 +674,19 @@
         <v>1820.28</v>
       </c>
       <c r="G8">
-        <v>-3989.17134</v>
+        <v>-3102.68882</v>
       </c>
       <c r="H8">
         <v>-0.1958193491851717</v>
       </c>
-      <c r="I8">
-        <v>32122</v>
-      </c>
-      <c r="J8">
-        <v>34138</v>
-      </c>
-      <c r="K8">
-        <v>2016</v>
+      <c r="I8" s="2">
+        <v>44367.89583333334</v>
+      </c>
+      <c r="J8" s="2">
+        <v>44374.89583333334</v>
+      </c>
+      <c r="K8" s="3">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -689,7 +694,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>34162</v>
@@ -704,19 +709,19 @@
         <v>2327.2</v>
       </c>
       <c r="G9">
-        <v>3013.451440000001</v>
+        <v>2636.770010000001</v>
       </c>
       <c r="H9">
         <v>0.1931186074275624</v>
       </c>
-      <c r="I9">
-        <v>34162</v>
-      </c>
-      <c r="J9">
-        <v>36178</v>
-      </c>
-      <c r="K9">
-        <v>2016</v>
+      <c r="I9" s="2">
+        <v>44374.97916666666</v>
+      </c>
+      <c r="J9" s="2">
+        <v>44381.97916666666</v>
+      </c>
+      <c r="K9" s="3">
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -724,7 +729,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>40857</v>
@@ -739,19 +744,19 @@
         <v>2298.26</v>
       </c>
       <c r="G10">
-        <v>4353.489500000005</v>
+        <v>3918.140550000005</v>
       </c>
       <c r="H10">
         <v>0.2336928271481349</v>
       </c>
-      <c r="I10">
-        <v>40857</v>
-      </c>
-      <c r="J10">
-        <v>42873</v>
-      </c>
-      <c r="K10">
-        <v>2016</v>
+      <c r="I10" s="2">
+        <v>44398.22569444445</v>
+      </c>
+      <c r="J10" s="2">
+        <v>44405.22569444445</v>
+      </c>
+      <c r="K10" s="3">
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -759,7 +764,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11">
         <v>44995</v>
@@ -774,19 +779,19 @@
         <v>3247.54</v>
       </c>
       <c r="G11">
-        <v>5638.334040000002</v>
+        <v>5011.852480000001</v>
       </c>
       <c r="H11">
         <v>0.2390185393958635</v>
       </c>
-      <c r="I11">
-        <v>44995</v>
-      </c>
-      <c r="J11">
-        <v>47011</v>
-      </c>
-      <c r="K11">
-        <v>2016</v>
+      <c r="I11" s="2">
+        <v>44412.59375</v>
+      </c>
+      <c r="J11" s="2">
+        <v>44419.59375</v>
+      </c>
+      <c r="K11" s="3">
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -814,14 +819,14 @@
       <c r="H12">
         <v>-0.06979643902398225</v>
       </c>
-      <c r="I12">
-        <v>53043</v>
-      </c>
-      <c r="J12">
-        <v>55059</v>
-      </c>
-      <c r="K12">
-        <v>2016</v>
+      <c r="I12" s="2">
+        <v>44440.72569444445</v>
+      </c>
+      <c r="J12" s="2">
+        <v>44447.72569444445</v>
+      </c>
+      <c r="K12" s="3">
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -829,7 +834,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13">
         <v>56117</v>
@@ -844,19 +849,19 @@
         <v>3362</v>
       </c>
       <c r="G13">
-        <v>-673.9423999999999</v>
+        <v>-589.6995999999999</v>
       </c>
       <c r="H13">
         <v>-0.02444482437511364</v>
       </c>
-      <c r="I13">
-        <v>56117</v>
-      </c>
-      <c r="J13">
-        <v>56760</v>
-      </c>
-      <c r="K13">
-        <v>643</v>
+      <c r="I13" s="2">
+        <v>44451.39930555555</v>
+      </c>
+      <c r="J13" s="2">
+        <v>44453.63194444445</v>
+      </c>
+      <c r="K13" s="3">
+        <v>2.232638888888889</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -864,7 +869,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14">
         <v>61577</v>
@@ -879,19 +884,19 @@
         <v>3628.03</v>
       </c>
       <c r="G14">
-        <v>3539.340560000004</v>
+        <v>3096.922990000004</v>
       </c>
       <c r="H14">
         <v>0.1388799107617749</v>
       </c>
-      <c r="I14">
-        <v>61577</v>
-      </c>
-      <c r="J14">
-        <v>63593</v>
-      </c>
-      <c r="K14">
-        <v>2016</v>
+      <c r="I14" s="2">
+        <v>44470.44097222222</v>
+      </c>
+      <c r="J14" s="2">
+        <v>44477.44097222222</v>
+      </c>
+      <c r="K14" s="3">
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -899,7 +904,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15">
         <v>67086</v>
@@ -914,19 +919,19 @@
         <v>4014.93</v>
       </c>
       <c r="G15">
-        <v>493.5666400000005</v>
+        <v>423.0571200000004</v>
       </c>
       <c r="H15">
         <v>0.01787576156180992</v>
       </c>
-      <c r="I15">
-        <v>67086</v>
-      </c>
-      <c r="J15">
-        <v>69102</v>
-      </c>
-      <c r="K15">
-        <v>2016</v>
+      <c r="I15" s="2">
+        <v>44489.56944444445</v>
+      </c>
+      <c r="J15" s="2">
+        <v>44496.56944444445</v>
+      </c>
+      <c r="K15" s="3">
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -934,7 +939,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16">
         <v>77682</v>
@@ -949,19 +954,19 @@
         <v>4547.54</v>
       </c>
       <c r="G16">
-        <v>2926.802900000001</v>
+        <v>2508.688200000001</v>
       </c>
       <c r="H16">
         <v>0.1012525156951016</v>
       </c>
-      <c r="I16">
-        <v>77682</v>
-      </c>
-      <c r="J16">
-        <v>79698</v>
-      </c>
-      <c r="K16">
-        <v>2016</v>
+      <c r="I16" s="2">
+        <v>44526.36111111111</v>
+      </c>
+      <c r="J16" s="2">
+        <v>44533.36111111111</v>
+      </c>
+      <c r="K16" s="3">
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -969,7 +974,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17">
         <v>79948</v>
@@ -984,19 +989,19 @@
         <v>4034.42</v>
       </c>
       <c r="G17">
-        <v>3270.353580000005</v>
+        <v>2906.980960000004</v>
       </c>
       <c r="H17">
         <v>0.09898336425175769</v>
       </c>
-      <c r="I17">
-        <v>79948</v>
-      </c>
-      <c r="J17">
-        <v>81964</v>
-      </c>
-      <c r="K17">
-        <v>2016</v>
+      <c r="I17" s="2">
+        <v>44534.22916666666</v>
+      </c>
+      <c r="J17" s="2">
+        <v>44541.22916666666</v>
+      </c>
+      <c r="K17" s="3">
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1004,34 +1009,34 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>-9</v>
+        <v>-8</v>
       </c>
       <c r="C18">
         <v>83291</v>
       </c>
       <c r="D18">
-        <v>89725</v>
+        <v>85307</v>
       </c>
       <c r="E18">
         <v>3987.91809</v>
       </c>
       <c r="F18">
-        <v>3218.51</v>
+        <v>3997.49</v>
       </c>
       <c r="G18">
-        <v>6924.672809999995</v>
+        <v>-76.57528000000093</v>
       </c>
       <c r="H18">
-        <v>0.1929347776548739</v>
-      </c>
-      <c r="I18">
-        <v>83291</v>
-      </c>
-      <c r="J18">
-        <v>89725</v>
-      </c>
-      <c r="K18">
-        <v>6434</v>
+        <v>-0.002400227332653104</v>
+      </c>
+      <c r="I18" s="2">
+        <v>44545.83680555555</v>
+      </c>
+      <c r="J18" s="2">
+        <v>44552.83680555555</v>
+      </c>
+      <c r="K18" s="3">
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1039,7 +1044,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C19">
         <v>89725</v>
@@ -1054,19 +1059,19 @@
         <v>3275.82</v>
       </c>
       <c r="G19">
-        <v>703.1893700000032</v>
+        <v>540.9149000000025</v>
       </c>
       <c r="H19">
         <v>0.01678958665576702</v>
       </c>
-      <c r="I19">
-        <v>89725</v>
-      </c>
-      <c r="J19">
-        <v>91741</v>
-      </c>
-      <c r="K19">
-        <v>2016</v>
+      <c r="I19" s="2">
+        <v>44568.17708333334</v>
+      </c>
+      <c r="J19" s="2">
+        <v>44575.17708333334</v>
+      </c>
+      <c r="K19" s="3">
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1074,7 +1079,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C20">
         <v>94695</v>
@@ -1089,19 +1094,19 @@
         <v>2536.15</v>
       </c>
       <c r="G20">
-        <v>5132.778940000008</v>
+        <v>3782.047640000006</v>
       </c>
       <c r="H20">
         <v>0.1192170406567823</v>
       </c>
-      <c r="I20">
-        <v>94695</v>
-      </c>
-      <c r="J20">
-        <v>96711</v>
-      </c>
-      <c r="K20">
-        <v>2016</v>
+      <c r="I20" s="2">
+        <v>44585.43402777778</v>
+      </c>
+      <c r="J20" s="2">
+        <v>44592.43402777778</v>
+      </c>
+      <c r="K20" s="3">
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1109,7 +1114,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C21">
         <v>97831</v>
@@ -1124,19 +1129,19 @@
         <v>3088.68</v>
       </c>
       <c r="G21">
-        <v>4782.022140000006</v>
+        <v>3656.840460000005</v>
       </c>
       <c r="H21">
         <v>0.1001983917714617</v>
       </c>
-      <c r="I21">
-        <v>97831</v>
-      </c>
-      <c r="J21">
-        <v>99847</v>
-      </c>
-      <c r="K21">
-        <v>2016</v>
+      <c r="I21" s="2">
+        <v>44596.32291666666</v>
+      </c>
+      <c r="J21" s="2">
+        <v>44603.32291666666</v>
+      </c>
+      <c r="K21" s="3">
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1144,7 +1149,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C22">
         <v>103543</v>
@@ -1159,19 +1164,19 @@
         <v>2900.53</v>
       </c>
       <c r="G22">
-        <v>10958.86000000001</v>
+        <v>7970.080000000009</v>
       </c>
       <c r="H22">
         <v>0.20734681984682</v>
       </c>
-      <c r="I22">
-        <v>103543</v>
-      </c>
-      <c r="J22">
-        <v>105559</v>
-      </c>
-      <c r="K22">
-        <v>2016</v>
+      <c r="I22" s="2">
+        <v>44616.15625</v>
+      </c>
+      <c r="J22" s="2">
+        <v>44623.15625</v>
+      </c>
+      <c r="K22" s="3">
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1179,7 +1184,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C23">
         <v>111040</v>
@@ -1194,19 +1199,19 @@
         <v>3388.49</v>
       </c>
       <c r="G23">
-        <v>7317.30279</v>
+        <v>5226.644850000001</v>
       </c>
       <c r="H23">
         <v>0.1146176321793129</v>
       </c>
-      <c r="I23">
-        <v>111040</v>
-      </c>
-      <c r="J23">
-        <v>113056</v>
-      </c>
-      <c r="K23">
-        <v>2016</v>
+      <c r="I23" s="2">
+        <v>44642.1875</v>
+      </c>
+      <c r="J23" s="2">
+        <v>44649.1875</v>
+      </c>
+      <c r="K23" s="3">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>